<commit_message>
Expanded ShipTester. Various small tweaks and bugfixes.
</commit_message>
<xml_diff>
--- a/notes/project notes.xlsx
+++ b/notes/project notes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="file format" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="279">
   <si>
     <t xml:space="preserve">FILES</t>
   </si>
@@ -571,6 +571,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">6</t>
     </r>
@@ -580,6 +581,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -588,6 +590,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -601,6 +604,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">5</t>
     </r>
@@ -610,6 +614,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -618,6 +623,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -649,6 +655,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">4</t>
     </r>
@@ -658,6 +665,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">th</t>
     </r>
@@ -666,6 +674,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -691,6 +700,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">3</t>
     </r>
@@ -700,6 +710,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">rd</t>
     </r>
@@ -708,6 +719,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -727,6 +739,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2</t>
     </r>
@@ -736,6 +749,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -744,6 +758,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -754,6 +769,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -763,6 +779,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">st</t>
     </r>
@@ -771,6 +788,7 @@
         <sz val="10.5"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> Rate</t>
     </r>
@@ -836,30 +854,51 @@
     <t xml:space="preserve">food</t>
   </si>
   <si>
+    <t xml:space="preserve">unmanned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drone</t>
+  </si>
+  <si>
     <t xml:space="preserve">solo</t>
   </si>
   <si>
+    <t xml:space="preserve">tiny</t>
+  </si>
+  <si>
     <t xml:space="preserve">heavy fighter</t>
   </si>
   <si>
+    <t xml:space="preserve">light</t>
+  </si>
+  <si>
     <t xml:space="preserve">cutter</t>
   </si>
   <si>
     <t xml:space="preserve">bomber</t>
   </si>
   <si>
+    <t xml:space="preserve">small</t>
+  </si>
+  <si>
     <t xml:space="preserve">corvette</t>
   </si>
   <si>
     <t xml:space="preserve">gunship</t>
   </si>
   <si>
+    <t xml:space="preserve">light shuttle</t>
+  </si>
+  <si>
     <t xml:space="preserve">destroyer/frigate</t>
   </si>
   <si>
     <t xml:space="preserve">cruiser</t>
   </si>
   <si>
+    <t xml:space="preserve">heavy shuttle</t>
+  </si>
+  <si>
     <t xml:space="preserve">assault ship</t>
   </si>
   <si>
@@ -891,9 +930,6 @@
   </si>
   <si>
     <t xml:space="preserve">CLASSIFICATION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drone</t>
   </si>
   <si>
     <t xml:space="preserve">PRIVATE</t>
@@ -1028,26 +1064,30 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10.5"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <vertAlign val="superscript"/>
       <sz val="10.5"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1183,7 +1223,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1228,6 +1268,14 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1236,7 +1284,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1264,7 +1312,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1272,24 +1320,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2683,8 +2719,8 @@
   </sheetPr>
   <dimension ref="B4:Q80"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L69" activeCellId="0" sqref="L69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A38" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L68" activeCellId="0" sqref="L68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2692,6 +2728,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="4.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="5.54"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.83"/>
   </cols>
   <sheetData>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2702,13 +2739,13 @@
       <c r="D4" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="8" t="s">
+      <c r="L4" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="N4" s="8" t="s">
+      <c r="N4" s="12" t="s">
         <v>157</v>
       </c>
-      <c r="P4" s="8" t="s">
+      <c r="P4" s="12" t="s">
         <v>156</v>
       </c>
     </row>
@@ -2716,13 +2753,13 @@
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
       <c r="D5" s="10"/>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="N5" s="8" t="s">
+      <c r="N5" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="P5" s="8" t="s">
+      <c r="P5" s="12" t="s">
         <v>158</v>
       </c>
     </row>
@@ -2730,148 +2767,148 @@
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="10"/>
-      <c r="L6" s="8" t="s">
+      <c r="L6" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="N6" s="8" t="s">
+      <c r="N6" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="P6" s="8" t="s">
+      <c r="P6" s="12" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="13" t="s">
         <v>163</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="L7" s="8" t="s">
+      <c r="L7" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="N7" s="8" t="s">
+      <c r="N7" s="12" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="11"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="13"/>
-      <c r="L8" s="8" t="s">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="L8" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="11"/>
-      <c r="C9" s="12" t="s">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14" t="s">
         <v>170</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="F9" s="8" t="s">
+      <c r="D9" s="15"/>
+      <c r="F9" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="L9" s="8" t="s">
+      <c r="L9" s="11" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="13"/>
-      <c r="L10" s="8" t="s">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="L10" s="11" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="11"/>
-      <c r="C11" s="14" t="s">
+      <c r="B11" s="13"/>
+      <c r="C11" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="D11" s="13"/>
-      <c r="F11" s="8" t="s">
+      <c r="D11" s="15"/>
+      <c r="F11" s="12" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="11"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="18" t="s">
         <v>164</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="15" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="15"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="13"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="15"/>
-      <c r="C15" s="17" t="s">
+      <c r="B15" s="17"/>
+      <c r="C15" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D15" s="13"/>
+      <c r="D15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="15"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="13"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="15"/>
-      <c r="C17" s="14" t="s">
+      <c r="B17" s="17"/>
+      <c r="C17" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="D17" s="13"/>
+      <c r="D17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="15"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="17"/>
+      <c r="C18" s="16"/>
+      <c r="D18" s="15"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="21" t="s">
         <v>178</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="15" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="13"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="18"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="13" t="s">
+      <c r="B21" s="20"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="15" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="18"/>
-      <c r="C22" s="19"/>
-      <c r="D22" s="13"/>
-      <c r="L22" s="8" t="s">
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="15"/>
+      <c r="L22" s="11" t="s">
         <v>181</v>
       </c>
       <c r="M22" s="0" t="n">
@@ -2879,498 +2916,524 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="D23" s="13" t="s">
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="L23" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="M23" s="20" t="str">
+      <c r="M23" s="22" t="str">
         <f aca="false">"2-4"</f>
         <v>2-4</v>
       </c>
-      <c r="P23" s="8" t="s">
+      <c r="P23" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="Q23" s="8" t="s">
+      <c r="Q23" s="12" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="18"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="13"/>
-      <c r="L24" s="8" t="s">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="15"/>
+      <c r="L24" s="11" t="s">
         <v>186</v>
       </c>
       <c r="M24" s="0" t="str">
         <f aca="false">"5-10"</f>
         <v>5-10</v>
       </c>
-      <c r="P24" s="8" t="s">
+      <c r="P24" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="Q24" s="8" t="s">
+      <c r="Q24" s="12" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="18"/>
-      <c r="C25" s="17" t="s">
+      <c r="B25" s="20"/>
+      <c r="C25" s="19" t="s">
         <v>189</v>
       </c>
-      <c r="D25" s="13" t="s">
+      <c r="D25" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="L25" s="11" t="s">
         <v>191</v>
       </c>
       <c r="M25" s="0" t="str">
         <f aca="false">"11+"</f>
         <v>11+</v>
       </c>
-      <c r="P25" s="8" t="s">
+      <c r="P25" s="12" t="s">
         <v>192</v>
       </c>
-      <c r="Q25" s="8" t="s">
+      <c r="Q25" s="12" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="18"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="13"/>
-      <c r="P26" s="8" t="s">
+      <c r="B26" s="20"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="15"/>
+      <c r="P26" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="Q26" s="8" t="s">
+      <c r="Q26" s="12" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="18"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="13" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="P27" s="8" t="s">
+      <c r="P27" s="12" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="18"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="13"/>
-      <c r="P28" s="8" t="s">
+      <c r="B28" s="20"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="15"/>
+      <c r="P28" s="12" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B29" s="18"/>
-      <c r="C29" s="21" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="23" t="s">
         <v>199</v>
       </c>
-      <c r="D29" s="13" t="s">
+      <c r="D29" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="P29" s="8" t="s">
+      <c r="P29" s="12" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="18"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="13"/>
+      <c r="B30" s="20"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="22" t="s">
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="24" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="18"/>
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D40" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6" t="s">
+      <c r="E40" s="1"/>
+      <c r="F40" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="G40" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="H40" s="6" t="s">
+      <c r="H40" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="I40" s="6" t="s">
+      <c r="I40" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="J40" s="6" t="s">
+      <c r="J40" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="K40" s="11" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C41" s="6" t="s">
+      <c r="C41" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="D41" s="6" t="s">
+      <c r="D41" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6" t="s">
+      <c r="E41" s="1"/>
+      <c r="F41" s="11" t="s">
         <v>209</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="G41" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="H41" s="6" t="s">
+      <c r="H41" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="I41" s="6" t="s">
+      <c r="I41" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="D42" s="6" t="s">
+      <c r="D42" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E42" s="6"/>
-      <c r="F42" s="6" t="s">
+      <c r="E42" s="1"/>
+      <c r="F42" s="11" t="s">
         <v>197</v>
       </c>
-      <c r="G42" s="6" t="s">
+      <c r="G42" s="11" t="s">
         <v>212</v>
       </c>
-      <c r="H42" s="6" t="s">
+      <c r="H42" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="I42" s="6" t="s">
+      <c r="I42" s="11" t="s">
         <v>214</v>
       </c>
-      <c r="J42" s="6"/>
-      <c r="K42" s="6"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C43" s="6" t="s">
+      <c r="C43" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6" t="s">
+      <c r="E43" s="1"/>
+      <c r="F43" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="G43" s="11" t="s">
         <v>195</v>
       </c>
-      <c r="H43" s="6" t="s">
+      <c r="H43" s="11" t="s">
         <v>215</v>
       </c>
-      <c r="I43" s="6" t="s">
+      <c r="I43" s="11" t="s">
         <v>216</v>
       </c>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="11" t="s">
         <v>217</v>
       </c>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6" t="s">
+      <c r="E44" s="1"/>
+      <c r="F44" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="G44" s="6"/>
-      <c r="H44" s="6" t="s">
+      <c r="G44" s="1"/>
+      <c r="H44" s="11" t="s">
         <v>218</v>
       </c>
-      <c r="I44" s="6" t="s">
+      <c r="I44" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="J44" s="6"/>
-      <c r="K44" s="6"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C45" s="6"/>
-      <c r="D45" s="6" t="s">
+      <c r="C45" s="1"/>
+      <c r="D45" s="11" t="s">
         <v>220</v>
       </c>
-      <c r="E45" s="6"/>
-      <c r="F45" s="6"/>
-      <c r="G45" s="6"/>
-      <c r="H45" s="6"/>
-      <c r="I45" s="6" t="s">
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="11" t="s">
         <v>221</v>
       </c>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6" t="s">
+      <c r="C46" s="1"/>
+      <c r="D46" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="6"/>
-      <c r="H46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="1"/>
+      <c r="G50" s="1"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
-      <c r="F51" s="6"/>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
-      <c r="G52" s="6"/>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="1"/>
+      <c r="G52" s="1"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-      <c r="H53" s="6"/>
-      <c r="I53" s="6"/>
-      <c r="J53" s="6"/>
-      <c r="K53" s="6"/>
+      <c r="F53" s="1"/>
+      <c r="G53" s="1"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F54" s="6"/>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6"/>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6"/>
-      <c r="K54" s="6"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F55" s="6"/>
-      <c r="G55" s="6"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="L60" s="6"/>
+      <c r="J60" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="K60" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L60" s="11" t="s">
+        <v>223</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="8" t="s">
+      <c r="D61" s="12" t="s">
         <v>171</v>
       </c>
       <c r="G61" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="H61" s="8" t="s">
+      <c r="H61" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="J61" s="23" t="s">
-        <v>222</v>
+      <c r="J61" s="25" t="s">
+        <v>224</v>
       </c>
       <c r="K61" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="L61" s="23" t="s">
+      <c r="L61" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="M61" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="M61" s="6"/>
+      <c r="N61" s="1"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="8" t="s">
+      <c r="D62" s="12" t="s">
         <v>188</v>
       </c>
       <c r="G62" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="H62" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="J62" s="23"/>
+      <c r="H62" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="J62" s="25"/>
       <c r="K62" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="L62" s="23" t="s">
+      <c r="L62" s="11" t="s">
+        <v>227</v>
+      </c>
+      <c r="M62" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="M62" s="6"/>
+      <c r="N62" s="1"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="8" t="s">
-        <v>224</v>
+      <c r="D63" s="12" t="s">
+        <v>228</v>
       </c>
       <c r="G63" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="H63" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="I63" s="8" t="s">
+      <c r="H63" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="I63" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="J63" s="23"/>
+      <c r="J63" s="25"/>
       <c r="K63" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="L63" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="M63" s="6"/>
+      <c r="L63" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="M63" s="11" t="s">
+        <v>226</v>
+      </c>
+      <c r="N63" s="1"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="8" t="s">
-        <v>226</v>
+      <c r="D64" s="12" t="s">
+        <v>231</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="H64" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="J64" s="23" t="s">
+      <c r="H64" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="J64" s="25" t="s">
         <v>183</v>
       </c>
       <c r="K64" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="L64" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="M64" s="6" t="s">
+      <c r="L64" s="11" t="s">
+        <v>233</v>
+      </c>
+      <c r="M64" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="N64" s="11" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="8" t="s">
-        <v>228</v>
+      <c r="D65" s="12" t="s">
+        <v>234</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="I65" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="J65" s="23"/>
+      <c r="I65" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="J65" s="25"/>
       <c r="K65" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="L65" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="M65" s="6"/>
+      <c r="L65" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="M65" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="N65" s="1"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="8" t="s">
-        <v>229</v>
+      <c r="D66" s="12" t="s">
+        <v>235</v>
       </c>
       <c r="G66" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="H66" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="J66" s="23"/>
+      <c r="H66" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="J66" s="25"/>
       <c r="K66" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="L66" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="M66" s="6" t="s">
+      <c r="L66" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="M66" s="11" t="s">
+        <v>237</v>
+      </c>
+      <c r="N66" s="11" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="8" t="s">
-        <v>231</v>
+      <c r="D67" s="12" t="s">
+        <v>238</v>
       </c>
       <c r="G67" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="H67" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="J67" s="23" t="s">
-        <v>233</v>
+      <c r="H67" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="J67" s="25" t="s">
+        <v>240</v>
       </c>
       <c r="K67" s="0" t="n">
         <v>7</v>
@@ -3380,155 +3443,155 @@
       <c r="G68" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="H68" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="J68" s="23"/>
+      <c r="H68" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="J68" s="25"/>
       <c r="K68" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="L68" s="6"/>
-      <c r="M68" s="6"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G69" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="J69" s="23"/>
+      <c r="H69" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="J69" s="25"/>
       <c r="K69" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="M69" s="6"/>
+      <c r="N69" s="1"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G70" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="H70" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="J70" s="23" t="s">
-        <v>226</v>
+      <c r="H70" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="J70" s="25" t="s">
+        <v>231</v>
       </c>
       <c r="K70" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="L70" s="6" t="s">
-        <v>224</v>
-      </c>
-      <c r="M70" s="6"/>
+      <c r="M70" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="N70" s="1"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G71" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="H71" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="J71" s="23"/>
+      <c r="H71" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="J71" s="25"/>
       <c r="K71" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="M71" s="6"/>
+      <c r="N71" s="1"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G72" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="H72" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="J72" s="23"/>
+      <c r="H72" s="12" t="s">
+        <v>245</v>
+      </c>
+      <c r="J72" s="25"/>
       <c r="K72" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="L72" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="M72" s="6"/>
+      <c r="M72" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="N72" s="1"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J73" s="23" t="s">
-        <v>232</v>
+      <c r="J73" s="25" t="s">
+        <v>239</v>
       </c>
       <c r="K73" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="L73" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="M73" s="6"/>
+      <c r="M73" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="N73" s="1"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J74" s="23"/>
+      <c r="J74" s="25"/>
       <c r="K74" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="M74" s="6"/>
+      <c r="N74" s="1"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J75" s="23"/>
+      <c r="J75" s="25"/>
       <c r="K75" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="L75" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="M75" s="6"/>
+      <c r="M75" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="N75" s="1"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J76" s="23" t="s">
-        <v>229</v>
+      <c r="J76" s="25" t="s">
+        <v>235</v>
       </c>
       <c r="K76" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="L76" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="M76" s="6"/>
+      <c r="M76" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="N76" s="1"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J77" s="23"/>
+      <c r="J77" s="25"/>
       <c r="K77" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="M77" s="6"/>
+      <c r="N77" s="1"/>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J78" s="23"/>
+      <c r="J78" s="25"/>
       <c r="K78" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="L78" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="M78" s="6"/>
+      <c r="M78" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="N78" s="1"/>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J79" s="23" t="s">
-        <v>231</v>
+      <c r="J79" s="25" t="s">
+        <v>238</v>
       </c>
       <c r="K79" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="L79" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="M79" s="6"/>
+      <c r="M79" s="11" t="s">
+        <v>244</v>
+      </c>
+      <c r="N79" s="1"/>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J80" s="23"/>
+      <c r="J80" s="25"/>
       <c r="K80" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="L80" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="M80" s="6"/>
+      <c r="M80" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="N80" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -3580,7 +3643,7 @@
   </sheetPr>
   <dimension ref="B3:K51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
@@ -3593,465 +3656,465 @@
   </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="24" t="s">
-        <v>239</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="F3" s="24" t="s">
-        <v>240</v>
-      </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+      <c r="B3" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="F3" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
       <c r="K3" s="8" t="str">
         <f aca="false">"FFF HPCC XXXX XXXX"</f>
         <v>FFF HPCC XXXX XXXX</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="24" t="n">
+      <c r="B4" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D4" s="25" t="s">
-        <v>241</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>242</v>
-      </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
+      <c r="D4" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F4" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="24" t="s">
-        <v>243</v>
+      <c r="B5" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="C5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="F5" s="24" t="s">
-        <v>244</v>
-      </c>
-      <c r="G5" s="24" t="n">
+      <c r="F5" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="G5" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="H5" s="24" t="n">
+      <c r="H5" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="25" t="s">
-        <v>245</v>
+      <c r="I5" s="12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="24" t="s">
-        <v>246</v>
+      <c r="B6" s="25" t="s">
+        <v>252</v>
       </c>
       <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="25" t="s">
-        <v>247</v>
+      <c r="I6" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="24" t="s">
-        <v>244</v>
+      <c r="B7" s="25" t="s">
+        <v>250</v>
       </c>
       <c r="C7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D7" s="25" t="s">
-        <v>226</v>
-      </c>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="F7" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="24" t="s">
-        <v>248</v>
+      <c r="B8" s="25" t="s">
+        <v>254</v>
       </c>
       <c r="C8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="F8" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="G8" s="24" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="24" t="n">
+      <c r="D8" s="12" t="s">
+        <v>239</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>254</v>
+      </c>
+      <c r="G8" s="25" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="25" t="s">
+      <c r="I8" s="12" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="24" t="s">
-        <v>249</v>
+      <c r="B9" s="25" t="s">
+        <v>255</v>
       </c>
       <c r="C9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="D9" s="25" t="s">
-        <v>234</v>
-      </c>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="D9" s="12" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I9" s="25" t="s">
-        <v>250</v>
+      <c r="I9" s="12" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="24" t="s">
-        <v>251</v>
+      <c r="B10" s="25" t="s">
+        <v>257</v>
       </c>
       <c r="C10" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="D10" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
+      <c r="D10" s="12" t="s">
+        <v>242</v>
+      </c>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
       <c r="H10" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="12" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="24" t="s">
-        <v>252</v>
+      <c r="B11" s="25" t="s">
+        <v>258</v>
       </c>
       <c r="C11" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="D11" s="25" t="s">
-        <v>236</v>
-      </c>
-      <c r="F11" s="24" t="s">
+      <c r="D11" s="12" t="s">
+        <v>243</v>
+      </c>
+      <c r="F11" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="24" t="s">
-        <v>253</v>
+      <c r="B12" s="25" t="s">
+        <v>259</v>
       </c>
       <c r="C12" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="D12" s="25" t="s">
-        <v>237</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>254</v>
-      </c>
-      <c r="G12" s="24" t="n">
+      <c r="D12" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>260</v>
+      </c>
+      <c r="G12" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="H12" s="24" t="n">
+      <c r="H12" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I12" s="25" t="s">
+      <c r="I12" s="12" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="24" t="s">
-        <v>255</v>
+      <c r="B13" s="25" t="s">
+        <v>261</v>
       </c>
       <c r="C13" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="D13" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
+      <c r="D13" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
       <c r="H13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I13" s="25" t="s">
+      <c r="I13" s="12" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
       <c r="H14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I14" s="25" t="s">
+      <c r="I14" s="12" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="0"/>
       <c r="C15" s="0"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
       <c r="H15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="25" t="s">
+      <c r="I15" s="12" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="24" t="s">
-        <v>257</v>
-      </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="F16" s="24" t="s">
-        <v>258</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="B16" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="F16" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="24" t="n">
+      <c r="B17" s="25" t="n">
         <v>0</v>
       </c>
       <c r="C17" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D17" s="25" t="s">
-        <v>259</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="G17" s="24" t="n">
-        <v>4</v>
-      </c>
-      <c r="H17" s="24" t="n">
+      <c r="D17" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="G17" s="25" t="n">
+        <v>4</v>
+      </c>
+      <c r="H17" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I17" s="25" t="s">
-        <v>261</v>
+      <c r="I17" s="12" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="24" t="s">
-        <v>243</v>
+      <c r="B18" s="25" t="s">
+        <v>249</v>
       </c>
       <c r="C18" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D18" s="25" t="s">
-        <v>262</v>
-      </c>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
+      <c r="D18" s="12" t="s">
+        <v>268</v>
+      </c>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
       <c r="H18" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I18" s="25" t="s">
+      <c r="I18" s="12" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="24" t="s">
-        <v>246</v>
+      <c r="B19" s="25" t="s">
+        <v>252</v>
       </c>
       <c r="C19" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="12" t="s">
         <v>159</v>
       </c>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
       <c r="H19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I19" s="25" t="s">
+      <c r="I19" s="12" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="24" t="s">
-        <v>244</v>
+      <c r="B20" s="25" t="s">
+        <v>250</v>
       </c>
       <c r="C20" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="12" t="s">
         <v>161</v>
       </c>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
       <c r="H20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I20" s="25" t="s">
+      <c r="I20" s="12" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="24" t="s">
-        <v>248</v>
+      <c r="B21" s="25" t="s">
+        <v>254</v>
       </c>
       <c r="C21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="F21" s="24" t="s">
-        <v>263</v>
-      </c>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="F21" s="25" t="s">
+        <v>269</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="0"/>
-      <c r="F22" s="24" t="s">
-        <v>264</v>
-      </c>
-      <c r="G22" s="24" t="n">
+      <c r="F22" s="25" t="s">
+        <v>270</v>
+      </c>
+      <c r="G22" s="25" t="n">
         <v>5</v>
       </c>
-      <c r="H22" s="24" t="n">
+      <c r="H22" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I22" s="25" t="s">
+      <c r="I22" s="12" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="0"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
+      <c r="F23" s="25"/>
+      <c r="G23" s="25"/>
       <c r="H23" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I23" s="25" t="s">
+      <c r="I23" s="12" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="0"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
       <c r="H24" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I24" s="25" t="s">
+      <c r="I24" s="12" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="0"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
       <c r="H25" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I25" s="25" t="s">
+      <c r="I25" s="12" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="0"/>
-      <c r="F26" s="24" t="s">
-        <v>265</v>
-      </c>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="F26" s="25" t="s">
+        <v>271</v>
+      </c>
+      <c r="G26" s="25"/>
+      <c r="H26" s="25"/>
+      <c r="I26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="0"/>
-      <c r="F27" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="G27" s="24" t="n">
+      <c r="F27" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="G27" s="25" t="n">
         <v>6</v>
       </c>
-      <c r="H27" s="24" t="n">
+      <c r="H27" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="I27" s="25" t="s">
-        <v>267</v>
+      <c r="I27" s="12" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
       <c r="H28" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I28" s="25" t="s">
-        <v>268</v>
+      <c r="I28" s="12" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="0"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
+      <c r="F29" s="25"/>
+      <c r="G29" s="25"/>
       <c r="H29" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I29" s="25" t="s">
+      <c r="I29" s="12" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
+      <c r="F30" s="25"/>
+      <c r="G30" s="25"/>
       <c r="H30" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I30" s="25" t="s">
-        <v>269</v>
+      <c r="I30" s="12" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F31" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
+      <c r="F31" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="G31" s="25"/>
+      <c r="H31" s="25"/>
+      <c r="I31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F32" s="26" t="s">
-        <v>271</v>
+      <c r="F32" s="11" t="s">
+        <v>277</v>
       </c>
       <c r="G32" s="1" t="n">
         <v>0</v>
@@ -4059,8 +4122,8 @@
       <c r="H32" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I32" s="25" t="s">
-        <v>272</v>
+      <c r="I32" s="12" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>